<commit_message>
se comenzo el marco teorico
</commit_message>
<xml_diff>
--- a/Referencias Consultadas Spreadsheet.xlsx
+++ b/Referencias Consultadas Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Documents\Universidad\TEG\Trabajo Especial de Grado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Desktop\TEG_JT_UCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83964997-AFD7-4223-BDED-0448755852B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19C37B4-0C22-427C-8E3B-4E5E52BAF6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Título</t>
   </si>
@@ -43,13 +43,151 @@
   </si>
   <si>
     <t>Notas</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Libro</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>Introducción a la Dinámica Estructural - Jorge Hurtado</t>
+  </si>
+  <si>
+    <t>En dinámica los elementos se rigen por sus grados de libertad. Se define la frecuencia natural y el amortiguamiento a partir de las ecuaciones diferenciales de movimiento.</t>
+  </si>
+  <si>
+    <t>Mecanica Vectorial para Ingenieros - Beer</t>
+  </si>
+  <si>
+    <t>Apuntes de Teoría de estructuras - U.Politecnica de Gijon</t>
+  </si>
+  <si>
+    <t>Definicion de estructura y caracteristicas generales. Tipos de Estrcuturas según su funcion estructural</t>
+  </si>
+  <si>
+    <t>2019/2020</t>
+  </si>
+  <si>
+    <t>Apuntes/Libro</t>
+  </si>
+  <si>
+    <t>ESTRUCTURAS 1 - Apuntes de Clase - Universidad de Cuenca</t>
+  </si>
+  <si>
+    <t>Tipos de estructuras. Pagina 280</t>
+  </si>
+  <si>
+    <t>Structural Analysis - Hibbeler</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Definiciones. Muy basico y poco profesional.</t>
+  </si>
+  <si>
+    <t>Definicion de estructura. Punto de vista arquitectónico.</t>
+  </si>
+  <si>
+    <t>https://textbooks.open.tudelft.nl/textbooks/catalog/book/15</t>
+  </si>
+  <si>
+    <t>Introduction to Aerospace Structures and Materials - Rene Alderliesten</t>
+  </si>
+  <si>
+    <t>Definiciones y principio de la estatica</t>
+  </si>
+  <si>
+    <t>Análisis estático de estructuras planas - Luisa Basset</t>
+  </si>
+  <si>
+    <t>https://m.riunet.upv.es/bitstream/handle/10251/38538/Análisis%20estático%20de%20estructuras%20planas%20.pdf?sequence=1&amp;isAllowed=y</t>
+  </si>
+  <si>
+    <t>Artículo</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Definicíón de comportamiento o respuesta estática y su importancia.</t>
+  </si>
+  <si>
+    <t>Artículo/Recopilación</t>
+  </si>
+  <si>
+    <t>http://www.vibrationdata.com/tutorials_alt/frf.pdf</t>
+  </si>
+  <si>
+    <t>Recopilación/Lectura Corta</t>
+  </si>
+  <si>
+    <t>An introduction to FRF - Tom Irvine Rapport, College of Engineering and Computer Science</t>
+  </si>
+  <si>
+    <t>BibTex Cite</t>
+  </si>
+  <si>
+    <t>https://scholar.googleusercontent.com/scholar.bib?q=info:VJUcDRz1qCIJ:scholar.google.com/&amp;output=citation&amp;scisdr=ClEKZ8IdEMnwzI08rZU:AFWwaeYAAAAAZRw6tZVbc_m38LsP-Zx41kiZcms&amp;scisig=AFWwaeYAAAAAZRw6tUuqHOwWkRUoq_EmC6flBi4&amp;scisf=4&amp;ct=citation&amp;cd=-1&amp;hl=es</t>
+  </si>
+  <si>
+    <t>Frecuencia natural en estrucutras e introduccion a la respuesta en frecuencia.</t>
+  </si>
+  <si>
+    <t>Damping Ratios of Reinforced Concrete Structures Under Actual Ground Motion Excitations</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-030-12115-0_36</t>
+  </si>
+  <si>
+    <t>Conference paper</t>
+  </si>
+  <si>
+    <t>Definicion de damping ratio.</t>
+  </si>
+  <si>
+    <t>https://community.sw.siemens.com/s/article/what-is-a-frequency-response-function-frf#:~:text=A%20Frequency%20Response%20Function%20(or,between%20the%20input%20and%20output</t>
+  </si>
+  <si>
+    <t>Artículo Web</t>
+  </si>
+  <si>
+    <t>What is a Frequency Response Function (FRF)? - Peter Schandelbrand SIEMENS</t>
+  </si>
+  <si>
+    <t>http://civilwares.free.fr/The%20Seismic%20Design%20Handbook/Chapter%2004-Dynamic%20Response%20of%20Buildings.pdf</t>
+  </si>
+  <si>
+    <t>Dynamic Response of Structures - James Anderson</t>
+  </si>
+  <si>
+    <t>Lectura general y breve sobre la respuesta en frecuencia aplicada a estructuras. Informacion util sobre la respuesta en frecuencia y la coherencia luego de medir sobre una estructura. Explicacion de formas modales y respuesta imaginaria.</t>
+  </si>
+  <si>
+    <t>Intro to SHM - Los Alamos Dynamics</t>
+  </si>
+  <si>
+    <t>Presentacion</t>
+  </si>
+  <si>
+    <t>DATO: For most structures, the amount of viscous damping in the system will vary between 3% and 10% of critical</t>
+  </si>
+  <si>
+    <t>Definición y causas del daño en una estrcutura.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,8 +208,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +224,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -112,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -121,6 +282,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,25 +618,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F67EF-8173-45AF-BC18-0B0A6EBE21A7}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="67.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,16 +646,298 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44936</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2007</v>
+      </c>
+      <c r="F3" s="4">
+        <v>44967</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <v>44967</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2014</v>
+      </c>
+      <c r="F5" s="4">
+        <v>44967</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2012</v>
+      </c>
+      <c r="F6" s="4">
+        <v>44967</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="F7" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2014</v>
+      </c>
+      <c r="F8" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F10" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F11" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2001</v>
+      </c>
+      <c r="F12" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4">
+        <v>44995</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avances en marco teorico
</commit_message>
<xml_diff>
--- a/Referencias Consultadas Spreadsheet.xlsx
+++ b/Referencias Consultadas Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Desktop\TEG_JT_UCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD0A6CB-69E0-49F0-B314-4328B15FF26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAF48A5-6CCD-458A-A75B-1C911B531931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
+    <workbookView xWindow="345" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +866,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
       <c r="B8" s="8" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
cambio en las citas a  formato APA sugerido
</commit_message>
<xml_diff>
--- a/Referencias Consultadas Spreadsheet.xlsx
+++ b/Referencias Consultadas Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Desktop\TEG_JT_UCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAF48A5-6CCD-458A-A75B-1C911B531931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3BE84C-AD09-4D5A-8FA0-FA34727D5051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,8 +677,8 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
antes de comenzar con salud estructural
</commit_message>
<xml_diff>
--- a/Referencias Consultadas Spreadsheet.xlsx
+++ b/Referencias Consultadas Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Desktop\TEG_JT_UCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3BE84C-AD09-4D5A-8FA0-FA34727D5051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672F3A2F-5C28-46AA-AE6D-06FE9C324322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>Título</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Structural Health Monitoring of Large Civil Structures - Chen</t>
   </si>
   <si>
-    <t xml:space="preserve">Definición, características, importancia y motivación del SHM. Arquitectura de un sistema SHM (pag 25). Estrategias/Metodos del SHM y justificación del uso de acelerómetros (p 26) </t>
-  </si>
-  <si>
     <t>14/10/2023</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Definición. Importancia del SHM. Tipos de SHM (Activa y Pasiva)</t>
   </si>
   <si>
-    <t>Origen del análisis de frecuencia natural y amortiguamiento. Por qué es importante medir variables ambientales (p. 53, 60, Conclusión 3). Redes de sensores inalámbricas, más económicas.  (p. 61, 62). Importancia de mediciones globales (p. 64)</t>
-  </si>
-  <si>
     <t>Structural healt monitoring History, applications and future Review Book - Mohamed Abdo</t>
   </si>
   <si>
@@ -229,6 +223,36 @@
   </si>
   <si>
     <t>.bib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definición, características, importancia y motivación del SHM. Arquitectura de un sistema SHM (pag 25). Estrategias/Metodos del SHM y justificación del uso de acelerómetros (p 26). Daño en estructuras civiles (p 100) </t>
+  </si>
+  <si>
+    <t>Modal-vibration-based Damage Identification - Worden</t>
+  </si>
+  <si>
+    <t>Articulo/Cap de libro</t>
+  </si>
+  <si>
+    <t>17/10/2023</t>
+  </si>
+  <si>
+    <t>Justificacion del analisis de frecuencia y amortiguamiento para fines de SHM. Problemas sobre mediciones erroneas producto de condiciones ambientales en la frecuencia natural.</t>
+  </si>
+  <si>
+    <t>Articulo</t>
+  </si>
+  <si>
+    <t>Modal Analysis for Damage Detection - Hearn</t>
+  </si>
+  <si>
+    <t>20/10/2023</t>
+  </si>
+  <si>
+    <t>Ecuaciones dinamicas que explican el por que se estudia el cambio en la frecuencia natural como indicativo de daño.</t>
+  </si>
+  <si>
+    <t>Origen del análisis de frecuencia natural y amortiguamiento, ecuaciones dinámicas. Por qué es importante medir variables ambientales (p. 53, 60, Conclusión 3). Redes de sensores inalámbricas, más económicas.  (p. 61, 62). Importancia de mediciones globales (p. 64)</t>
   </si>
 </sst>
 </file>
@@ -674,11 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F67EF-8173-45AF-BC18-0B0A6EBE21A7}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +721,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1048,10 +1072,10 @@
         <v>2007</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1075,12 +1099,12 @@
         <v>45148</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="57.75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="57.75" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1095,15 +1119,15 @@
         <v>2006</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1118,18 +1142,19 @@
         <v>2006</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
@@ -1141,10 +1166,54 @@
         <v>2014</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2009</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1991</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lista la parte de Salud Estructural
</commit_message>
<xml_diff>
--- a/Referencias Consultadas Spreadsheet.xlsx
+++ b/Referencias Consultadas Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatov\Desktop\TEG_JT_UCV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FF73B2-6782-4E03-B3B9-6431EB1123B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0141E9-7A10-4896-B6FE-AD0F9832A2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5898B617-1D6E-4B4F-93AC-B192439AA122}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Título</t>
   </si>
@@ -294,10 +294,22 @@
     <t>Justificacion en la medicion de inclinacion.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bridge-Deflection Estimation through Inclinometer Data Considering Structural Damages - </t>
-  </si>
-  <si>
     <t>Justificacion en la medicion de inclinacion/desplazamiento.</t>
+  </si>
+  <si>
+    <t>Bridge-Deflection Estimation through Inclinometer Data Considering Structural Damages - Zhang</t>
+  </si>
+  <si>
+    <t>28/10/2023</t>
+  </si>
+  <si>
+    <t>Definición breve y ventajas de los smart sensors.</t>
+  </si>
+  <si>
+    <t>Introduction to Instrumentation, Sensors and Process Control - Dunn</t>
+  </si>
+  <si>
+    <t>Sensor Technologies for Civil Infrastructure</t>
   </si>
 </sst>
 </file>
@@ -752,11 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F67EF-8173-45AF-BC18-0B0A6EBE21A7}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1392,9 @@
       <c r="D26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F26" s="3">
         <v>2023</v>
       </c>
@@ -1392,8 +1406,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="72" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
       <c r="B27" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
@@ -1401,6 +1416,9 @@
       <c r="D27" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E27" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="F27" s="3">
         <v>2017</v>
       </c>
@@ -1408,7 +1426,47 @@
         <v>85</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2006</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>